<commit_message>
minor bugfix in metadata
</commit_message>
<xml_diff>
--- a/research/links.xlsx
+++ b/research/links.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Uni\Semester_3\masterarbeit-julian\research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Uni\Semester_3\vSLAM-eval\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91185289-8395-41B1-8E30-A15D06FC1F69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CA1A1E-503B-451D-AF36-F00DBFD79DDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -565,7 +565,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B9" t="s">
@@ -598,6 +598,7 @@
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1" xr:uid="{E2108549-91DF-4D4C-B7B3-D4A4BC1EF938}"/>
     <hyperlink ref="A5" r:id="rId2" xr:uid="{A4C8126F-0487-4127-9377-8F33FC406AAB}"/>
+    <hyperlink ref="A9" r:id="rId3" xr:uid="{ECE541B1-1456-49BC-9F4B-DE161ABEDB57}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
integrated dsm slam into the run-script
</commit_message>
<xml_diff>
--- a/research/links.xlsx
+++ b/research/links.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Uni\Semester_3\vSLAM-eval\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CA1A1E-503B-451D-AF36-F00DBFD79DDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA633AED-5ACE-4277-9A86-CF4BF0667AC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>link</t>
   </si>
@@ -109,6 +118,24 @@
   </si>
   <si>
     <t>wie mache ich die evaluation</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/337638775_MAPPING_QUALITY_EVALUATION_OF_MONOCULAR_SLAM_SOLUTIONS_FOR_MICRO_AERIAL_VEHICLES/fulltext/5de1c01e299bf10bc33147f9/MAPPING-QUALITY-EVALUATION-OF-MONOCULAR-SLAM-SOLUTIONS-FOR-MICRO-AERIAL-VEHICLES.pdf</t>
+  </si>
+  <si>
+    <t>point cloud comparison</t>
+  </si>
+  <si>
+    <t>wurde nicht oft gemacht</t>
+  </si>
+  <si>
+    <t>https://www.hindawi.com/journals/js/2021/2054828/</t>
+  </si>
+  <si>
+    <t>vergleich 2021</t>
+  </si>
+  <si>
+    <t>gute übersicht über einzelne methoden</t>
   </si>
 </sst>
 </file>
@@ -446,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -540,7 +567,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B7" t="s">
@@ -578,8 +605,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="12" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -599,6 +652,9 @@
     <hyperlink ref="A6" r:id="rId1" xr:uid="{E2108549-91DF-4D4C-B7B3-D4A4BC1EF938}"/>
     <hyperlink ref="A5" r:id="rId2" xr:uid="{A4C8126F-0487-4127-9377-8F33FC406AAB}"/>
     <hyperlink ref="A9" r:id="rId3" xr:uid="{ECE541B1-1456-49BC-9F4B-DE161ABEDB57}"/>
+    <hyperlink ref="A10" r:id="rId4" xr:uid="{E5FCBA6D-A204-41EF-AE55-B8D8C905CCD9}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{802E3554-5FA6-454E-83FA-C3C896C0BFD1}"/>
+    <hyperlink ref="A11" r:id="rId6" xr:uid="{C1063ACE-A2AD-406C-B6E6-7F697D4C4E10}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added point cloud analysis
</commit_message>
<xml_diff>
--- a/research/links.xlsx
+++ b/research/links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Uni\Semester_3\vSLAM-eval\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA633AED-5ACE-4277-9A86-CF4BF0667AC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73083042-A54B-4C15-9E5C-BC947D587932}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>